<commit_message>
Put connectionString in config.json and changed all new DatabaseContext to _db
</commit_message>
<xml_diff>
--- a/Ferienliste_Technik.xlsx
+++ b/Ferienliste_Technik.xlsx
@@ -235,7 +235,7 @@
       </c>
       <c r="B2">
         <f>B5/B3</f>
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -246,13 +246,13 @@
     <row r="4">
       <c r="B4">
         <f>B3-B5</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
       <c r="B5">
         <f>SUM(B6:B58)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -668,7 +668,7 @@
         <v>52</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">

</xml_diff>